<commit_message>
Remove vessel density results CSV, update project metadata and add new image entries, and create a new Groovy script for distance calculations.
</commit_message>
<xml_diff>
--- a/Groups.xlsx
+++ b/Groups.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
   <si>
     <t xml:space="preserve">ALT ID</t>
   </si>
@@ -38,118 +38,127 @@
     <t xml:space="preserve">qupath: ~/SpleeenFollicleCounterQP, D6-36LinuxTopShelf</t>
   </si>
   <si>
+    <t xml:space="preserve">hipergator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/run/user/1001/gvfs/smb-share:server=path.ahc.ufl.edu,share=path$/PERSONAL/smith6jt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-25panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T/T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDL073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBMP004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLADR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRS1_Percentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRS2_Percentile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA_GRS</t>
+  </si>
+  <si>
     <t xml:space="preserve">qupath: ~\NCOMMS_master\QuPath_Spleen2025Aug1, D6-36Win11TopShelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hipergator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C/C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C/T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x-25panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T/T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBMP004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLADR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRS1_Percentile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRS2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRS2_Percentile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AA_GRS</t>
   </si>
   <si>
     <t xml:space="preserve">DRX/X</t>
@@ -260,14 +269,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -305,7 +314,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,15 +331,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,7 +355,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,7 +367,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,10 +563,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD41"/>
+  <dimension ref="A1:XFD42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26:E26"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,7 +575,6 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -581,9 +597,6 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -633,7 +646,7 @@
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -651,9 +664,6 @@
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -701,7 +711,7 @@
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -712,13 +722,16 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E12" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="G12" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -729,10 +742,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
@@ -743,15 +756,12 @@
         <v>2006</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="0" t="s">
         <v>9</v>
       </c>
     </row>
@@ -760,107 +770,101 @@
         <v>2007</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>29</v>
+      <c r="E17" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="E19" s="6"/>
+      <c r="G19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>1902</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-    </row>
-    <row r="24" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="XEW24" s="0"/>
-      <c r="XEX24" s="0"/>
-      <c r="XEY24" s="0"/>
-      <c r="XEZ24" s="0"/>
-      <c r="XFA24" s="0"/>
-      <c r="XFB24" s="0"/>
-      <c r="XFC24" s="0"/>
-      <c r="XFD24" s="0"/>
-    </row>
-    <row r="25" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>1901</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+    </row>
+    <row r="25" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="XEU25" s="0"/>
+      <c r="XEV25" s="0"/>
       <c r="XEW25" s="0"/>
       <c r="XEX25" s="0"/>
       <c r="XEY25" s="0"/>
@@ -871,10 +875,12 @@
       <c r="XFD25" s="0"/>
     </row>
     <row r="26" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="XEU26" s="0"/>
+      <c r="XEV26" s="0"/>
       <c r="XEW26" s="0"/>
       <c r="XEX26" s="0"/>
       <c r="XEY26" s="0"/>
@@ -885,10 +891,12 @@
       <c r="XFD26" s="0"/>
     </row>
     <row r="27" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="XEU27" s="0"/>
+      <c r="XEV27" s="0"/>
       <c r="XEW27" s="0"/>
       <c r="XEX27" s="0"/>
       <c r="XEY27" s="0"/>
@@ -899,10 +907,12 @@
       <c r="XFD27" s="0"/>
     </row>
     <row r="28" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="XEU28" s="0"/>
+      <c r="XEV28" s="0"/>
       <c r="XEW28" s="0"/>
       <c r="XEX28" s="0"/>
       <c r="XEY28" s="0"/>
@@ -915,8 +925,10 @@
     <row r="29" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="7"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="8"/>
+      <c r="XEU29" s="0"/>
+      <c r="XEV29" s="0"/>
       <c r="XEW29" s="0"/>
       <c r="XEX29" s="0"/>
       <c r="XEY29" s="0"/>
@@ -927,10 +939,12 @@
       <c r="XFD29" s="0"/>
     </row>
     <row r="30" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="XEU30" s="0"/>
+      <c r="XEV30" s="0"/>
       <c r="XEW30" s="0"/>
       <c r="XEX30" s="0"/>
       <c r="XEY30" s="0"/>
@@ -941,10 +955,12 @@
       <c r="XFD30" s="0"/>
     </row>
     <row r="31" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="XEU31" s="0"/>
+      <c r="XEV31" s="0"/>
       <c r="XEW31" s="0"/>
       <c r="XEX31" s="0"/>
       <c r="XEY31" s="0"/>
@@ -955,10 +971,12 @@
       <c r="XFD31" s="0"/>
     </row>
     <row r="32" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="XEU32" s="0"/>
+      <c r="XEV32" s="0"/>
       <c r="XEW32" s="0"/>
       <c r="XEX32" s="0"/>
       <c r="XEY32" s="0"/>
@@ -969,10 +987,12 @@
       <c r="XFD32" s="0"/>
     </row>
     <row r="33" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="XEU33" s="0"/>
+      <c r="XEV33" s="0"/>
       <c r="XEW33" s="0"/>
       <c r="XEX33" s="0"/>
       <c r="XEY33" s="0"/>
@@ -983,10 +1003,12 @@
       <c r="XFD33" s="0"/>
     </row>
     <row r="34" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="XEU34" s="0"/>
+      <c r="XEV34" s="0"/>
       <c r="XEW34" s="0"/>
       <c r="XEX34" s="0"/>
       <c r="XEY34" s="0"/>
@@ -997,10 +1019,12 @@
       <c r="XFD34" s="0"/>
     </row>
     <row r="35" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="XEU35" s="0"/>
+      <c r="XEV35" s="0"/>
       <c r="XEW35" s="0"/>
       <c r="XEX35" s="0"/>
       <c r="XEY35" s="0"/>
@@ -1011,10 +1035,12 @@
       <c r="XFD35" s="0"/>
     </row>
     <row r="36" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="XEU36" s="0"/>
+      <c r="XEV36" s="0"/>
       <c r="XEW36" s="0"/>
       <c r="XEX36" s="0"/>
       <c r="XEY36" s="0"/>
@@ -1025,10 +1051,12 @@
       <c r="XFD36" s="0"/>
     </row>
     <row r="37" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="XEU37" s="0"/>
+      <c r="XEV37" s="0"/>
       <c r="XEW37" s="0"/>
       <c r="XEX37" s="0"/>
       <c r="XEY37" s="0"/>
@@ -1039,10 +1067,12 @@
       <c r="XFD37" s="0"/>
     </row>
     <row r="38" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="XEU38" s="0"/>
+      <c r="XEV38" s="0"/>
       <c r="XEW38" s="0"/>
       <c r="XEX38" s="0"/>
       <c r="XEY38" s="0"/>
@@ -1053,10 +1083,12 @@
       <c r="XFD38" s="0"/>
     </row>
     <row r="39" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="XEU39" s="0"/>
+      <c r="XEV39" s="0"/>
       <c r="XEW39" s="0"/>
       <c r="XEX39" s="0"/>
       <c r="XEY39" s="0"/>
@@ -1066,11 +1098,13 @@
       <c r="XFC39" s="0"/>
       <c r="XFD39" s="0"/>
     </row>
-    <row r="40" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+    <row r="40" s="6" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="XEU40" s="0"/>
+      <c r="XEV40" s="0"/>
       <c r="XEW40" s="0"/>
       <c r="XEX40" s="0"/>
       <c r="XEY40" s="0"/>
@@ -1081,10 +1115,12 @@
       <c r="XFD40" s="0"/>
     </row>
     <row r="41" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="XEU41" s="0"/>
+      <c r="XEV41" s="0"/>
       <c r="XEW41" s="0"/>
       <c r="XEX41" s="0"/>
       <c r="XEY41" s="0"/>
@@ -1093,6 +1129,22 @@
       <c r="XFB41" s="0"/>
       <c r="XFC41" s="0"/>
       <c r="XFD41" s="0"/>
+    </row>
+    <row r="42" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="XEU42" s="0"/>
+      <c r="XEV42" s="0"/>
+      <c r="XEW42" s="0"/>
+      <c r="XEX42" s="0"/>
+      <c r="XEY42" s="0"/>
+      <c r="XEZ42" s="0"/>
+      <c r="XFA42" s="0"/>
+      <c r="XFB42" s="0"/>
+      <c r="XFC42" s="0"/>
+      <c r="XFD42" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1113,7 +1165,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D26:E26 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1142,25 +1194,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
@@ -1168,8 +1220,8 @@
       <c r="M1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>5</v>
+      <c r="N1" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>4</v>
@@ -1180,7 +1232,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>8</v>
@@ -1212,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>2.51</v>
@@ -1244,7 +1296,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0.26</v>
@@ -1301,7 +1353,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2.88</v>
@@ -1318,7 +1370,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>9.44</v>
@@ -1341,7 +1393,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>1.59</v>
@@ -1370,7 +1422,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>0</v>
@@ -1399,10 +1451,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>1.52</v>
@@ -1416,10 +1468,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>18</v>
@@ -1430,7 +1482,7 @@
         <v>2006</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>18</v>
@@ -1444,7 +1496,7 @@
         <v>2007</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>18</v>
@@ -1452,10 +1504,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>10</v>
@@ -1464,15 +1516,15 @@
         <v>18</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>8</v>
@@ -1481,16 +1533,16 @@
         <v>18</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>1.74</v>
@@ -1511,7 +1563,7 @@
         <v>6.12</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M20" s="0" t="s">
         <v>9</v>
@@ -1522,16 +1574,16 @@
         <v>1902</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>9</v>
@@ -1542,13 +1594,13 @@
         <v>1901</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,44 +1632,44 @@
       <c r="L24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
+      <c r="A25" s="12"/>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="11" t="s">
-        <v>55</v>
+      <c r="D30" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,10 +1677,10 @@
         <v>2009</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>